<commit_message>
ruff formated all files and renamed run_intertemporal_solar file to run_urbs_extension
</commit_message>
<xml_diff>
--- a/Input_urbsextensionv1.xlsx
+++ b/Input_urbsextensionv1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gerald\Desktop\urbsextension\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxoi\GitHub\urbs-extension\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{128E7585-C206-4725-9DE7-6476AEADA30F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E42B94D9-F7A9-4F57-AF86-552E387DCA71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{81864710-3A67-40FC-ABA1-4EF02E4F8A12}"/>
+    <workbookView xWindow="67200" yWindow="-570" windowWidth="28800" windowHeight="15285" activeTab="4" xr2:uid="{81864710-3A67-40FC-ABA1-4EF02E4F8A12}"/>
   </bookViews>
   <sheets>
     <sheet name="Base" sheetId="10" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="41">
   <si>
     <t>Value</t>
   </si>
@@ -145,6 +145,27 @@
   </si>
   <si>
     <t>timestep</t>
+  </si>
+  <si>
+    <t>scrap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mining </t>
+  </si>
+  <si>
+    <t>recycling_efficiency</t>
+  </si>
+  <si>
+    <t>recycling_EU27_solarPV</t>
+  </si>
+  <si>
+    <t>recycling_EU27_windoff</t>
+  </si>
+  <si>
+    <t>IR_recycling</t>
+  </si>
+  <si>
+    <t>Initial_decommisions</t>
   </si>
 </sst>
 </file>
@@ -656,9 +677,9 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -666,7 +687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -674,7 +695,7 @@
         <v>2024</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -682,7 +703,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -697,20 +718,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6185AF38-42FD-4CFF-B287-2FCFFF6C6EF3}">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:F28"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
-    <col min="3" max="3" width="26.7109375" customWidth="1"/>
-    <col min="4" max="4" width="37.28515625" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" customWidth="1"/>
+    <col min="3" max="3" width="26.6640625" customWidth="1"/>
+    <col min="4" max="4" width="37.33203125" customWidth="1"/>
+    <col min="9" max="9" width="22.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -724,16 +746,22 @@
         <v>23</v>
       </c>
       <c r="E1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" t="s">
         <v>28</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>29</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2024</v>
       </c>
@@ -747,16 +775,22 @@
         <v>414000</v>
       </c>
       <c r="E2">
+        <v>50000</v>
+      </c>
+      <c r="F2">
         <v>250240</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>303600</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>600000</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I2">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2025</v>
       </c>
@@ -770,16 +804,22 @@
         <v>414000</v>
       </c>
       <c r="E3">
+        <v>50000</v>
+      </c>
+      <c r="F3">
         <v>246486.39999999999</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>299045.40000000002</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>600000</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I3">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2026</v>
       </c>
@@ -793,16 +833,22 @@
         <v>414000</v>
       </c>
       <c r="E4">
+        <v>50000</v>
+      </c>
+      <c r="F4">
         <v>242789.10399999999</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>294559.71899999998</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>600000</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I4">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2027</v>
       </c>
@@ -816,16 +862,22 @@
         <v>414000</v>
       </c>
       <c r="E5">
+        <v>50000</v>
+      </c>
+      <c r="F5">
         <v>239147.26740000001</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>290141.32319999998</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>600000</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I5">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2028</v>
       </c>
@@ -839,16 +891,22 @@
         <v>414000</v>
       </c>
       <c r="E6">
+        <v>50000</v>
+      </c>
+      <c r="F6">
         <v>235560.05840000001</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>285788.2034</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>600000</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I6">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2029</v>
       </c>
@@ -862,16 +920,22 @@
         <v>414000</v>
       </c>
       <c r="E7">
+        <v>50000</v>
+      </c>
+      <c r="F7">
         <v>232026.65760000001</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>281498.4804</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>600000</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I7">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2030</v>
       </c>
@@ -885,16 +949,22 @@
         <v>414000</v>
       </c>
       <c r="E8">
+        <v>50000</v>
+      </c>
+      <c r="F8">
         <v>228546.25769999999</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>277270.34419999999</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>600000</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I8">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2031</v>
       </c>
@@ -908,16 +978,22 @@
         <v>414000</v>
       </c>
       <c r="E9">
+        <v>50000</v>
+      </c>
+      <c r="F9">
         <v>225118.0638</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>273102.28909999999</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>600000</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I9">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2032</v>
       </c>
@@ -931,16 +1007,22 @@
         <v>414000</v>
       </c>
       <c r="E10">
+        <v>50000</v>
+      </c>
+      <c r="F10">
         <v>221741.2929</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>268993.2548</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>600000</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I10">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2033</v>
       </c>
@@ -954,16 +1036,22 @@
         <v>414000</v>
       </c>
       <c r="E11">
+        <v>50000</v>
+      </c>
+      <c r="F11">
         <v>218415.1735</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>264942.41499999998</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>600000</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I11">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2034</v>
       </c>
@@ -977,16 +1065,22 @@
         <v>414000</v>
       </c>
       <c r="E12">
+        <v>50000</v>
+      </c>
+      <c r="F12">
         <v>215138.94589999999</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>260948.7948</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>600000</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I12">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2035</v>
       </c>
@@ -1000,16 +1094,22 @@
         <v>414000</v>
       </c>
       <c r="E13">
+        <v>50000</v>
+      </c>
+      <c r="F13">
         <v>211911.86170000001</v>
       </c>
-      <c r="F13">
+      <c r="G13">
         <v>257011.4613</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <v>600000</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I13">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2036</v>
       </c>
@@ -1023,16 +1123,22 @@
         <v>414000</v>
       </c>
       <c r="E14">
+        <v>50000</v>
+      </c>
+      <c r="F14">
         <v>208733.1838</v>
       </c>
-      <c r="F14">
+      <c r="G14">
         <v>253129.39139999999</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <v>600000</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I14">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2037</v>
       </c>
@@ -1046,16 +1152,22 @@
         <v>414000</v>
       </c>
       <c r="E15">
+        <v>50000</v>
+      </c>
+      <c r="F15">
         <v>205602.18599999999</v>
       </c>
-      <c r="F15">
+      <c r="G15">
         <v>249301.63759999999</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <v>600000</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I15">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2038</v>
       </c>
@@ -1069,16 +1181,22 @@
         <v>414000</v>
       </c>
       <c r="E16">
+        <v>50000</v>
+      </c>
+      <c r="F16">
         <v>202518.1532</v>
       </c>
-      <c r="F16">
+      <c r="G16">
         <v>245527.30809999999</v>
       </c>
-      <c r="G16">
+      <c r="H16">
         <v>600000</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I16">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2039</v>
       </c>
@@ -1092,16 +1210,22 @@
         <v>414000</v>
       </c>
       <c r="E17">
+        <v>50000</v>
+      </c>
+      <c r="F17">
         <v>199480.38089999999</v>
       </c>
-      <c r="F17">
+      <c r="G17">
         <v>241805.39859999999</v>
       </c>
-      <c r="G17">
+      <c r="H17">
         <v>600000</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I17">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2040</v>
       </c>
@@ -1115,16 +1239,22 @@
         <v>414000</v>
       </c>
       <c r="E18">
+        <v>50000</v>
+      </c>
+      <c r="F18">
         <v>196488.1752</v>
       </c>
-      <c r="F18">
+      <c r="G18">
         <v>238134.9901</v>
       </c>
-      <c r="G18">
+      <c r="H18">
         <v>600000</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I18">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2041</v>
       </c>
@@ -1138,16 +1268,22 @@
         <v>414000</v>
       </c>
       <c r="E19">
+        <v>50000</v>
+      </c>
+      <c r="F19">
         <v>193540.85260000001</v>
       </c>
-      <c r="F19">
+      <c r="G19">
         <v>234515.065</v>
       </c>
-      <c r="G19">
+      <c r="H19">
         <v>600000</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I19">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2042</v>
       </c>
@@ -1161,16 +1297,22 @@
         <v>414000</v>
       </c>
       <c r="E20">
+        <v>50000</v>
+      </c>
+      <c r="F20">
         <v>190637.73980000001</v>
       </c>
-      <c r="F20">
+      <c r="G20">
         <v>230944.68799999999</v>
       </c>
-      <c r="G20">
+      <c r="H20">
         <v>600000</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I20">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>2043</v>
       </c>
@@ -1184,16 +1326,22 @@
         <v>414000</v>
       </c>
       <c r="E21">
+        <v>50000</v>
+      </c>
+      <c r="F21">
         <v>187778.17370000001</v>
       </c>
-      <c r="F21">
+      <c r="G21">
         <v>227422.96530000001</v>
       </c>
-      <c r="G21">
+      <c r="H21">
         <v>600000</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I21">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>2044</v>
       </c>
@@ -1207,16 +1355,22 @@
         <v>414000</v>
       </c>
       <c r="E22">
+        <v>50000</v>
+      </c>
+      <c r="F22">
         <v>184961.50109999999</v>
       </c>
-      <c r="F22">
+      <c r="G22">
         <v>223948.88099999999</v>
       </c>
-      <c r="G22">
+      <c r="H22">
         <v>600000</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I22">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>2045</v>
       </c>
@@ -1230,16 +1384,22 @@
         <v>414000</v>
       </c>
       <c r="E23">
+        <v>50000</v>
+      </c>
+      <c r="F23">
         <v>182187.07860000001</v>
       </c>
-      <c r="F23">
+      <c r="G23">
         <v>220521.46350000001</v>
       </c>
-      <c r="G23">
+      <c r="H23">
         <v>600000</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I23">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>2046</v>
       </c>
@@ -1253,16 +1413,22 @@
         <v>414000</v>
       </c>
       <c r="E24">
+        <v>50000</v>
+      </c>
+      <c r="F24">
         <v>179454.27239999999</v>
       </c>
-      <c r="F24">
+      <c r="G24">
         <v>217139.74350000001</v>
       </c>
-      <c r="G24">
+      <c r="H24">
         <v>600000</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I24">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>2047</v>
       </c>
@@ -1276,16 +1442,22 @@
         <v>414000</v>
       </c>
       <c r="E25">
+        <v>50000</v>
+      </c>
+      <c r="F25">
         <v>176762.4583</v>
       </c>
-      <c r="F25">
+      <c r="G25">
         <v>213802.75769999999</v>
       </c>
-      <c r="G25">
+      <c r="H25">
         <v>600000</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I25">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>2048</v>
       </c>
@@ -1299,16 +1471,22 @@
         <v>414000</v>
       </c>
       <c r="E26">
+        <v>50000</v>
+      </c>
+      <c r="F26">
         <v>174111.0214</v>
       </c>
-      <c r="F26">
+      <c r="G26">
         <v>210509.61679999999</v>
       </c>
-      <c r="G26">
+      <c r="H26">
         <v>600000</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I26">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>2049</v>
       </c>
@@ -1322,16 +1500,22 @@
         <v>414000</v>
       </c>
       <c r="E27">
+        <v>50000</v>
+      </c>
+      <c r="F27">
         <v>171499.3561</v>
       </c>
-      <c r="F27">
+      <c r="G27">
         <v>207259.3126</v>
       </c>
-      <c r="G27">
+      <c r="H27">
         <v>600000</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I27">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>2050</v>
       </c>
@@ -1345,13 +1529,19 @@
         <v>414000</v>
       </c>
       <c r="E28">
+        <v>50000</v>
+      </c>
+      <c r="F28">
         <v>168926.8658</v>
       </c>
-      <c r="F28">
+      <c r="G28">
         <v>204050.9535</v>
       </c>
-      <c r="G28">
+      <c r="H28">
         <v>600000</v>
+      </c>
+      <c r="I28">
+        <v>50000</v>
       </c>
     </row>
   </sheetData>
@@ -1367,64 +1557,64 @@
       <selection activeCell="C1" sqref="C1:H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" customWidth="1"/>
+    <col min="1" max="1" width="17.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" s="5"/>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" s="5"/>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" s="5"/>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" s="5"/>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" s="5"/>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" s="5"/>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" s="5"/>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" s="5"/>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" s="5"/>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="5"/>
     </row>
   </sheetData>
@@ -1436,16 +1626,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6341E4C-4AB4-44A4-8119-B6BB3BEB6E84}">
   <dimension ref="A1:D325"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="17.7109375" customWidth="1"/>
+    <col min="4" max="4" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -1459,7 +1649,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1473,7 +1663,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1487,7 +1677,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1501,7 +1691,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1515,7 +1705,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1529,7 +1719,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1543,7 +1733,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1557,7 +1747,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1571,7 +1761,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1585,7 +1775,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1599,7 +1789,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1613,7 +1803,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1627,7 +1817,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>1</v>
       </c>
@@ -1641,7 +1831,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2</v>
       </c>
@@ -1655,7 +1845,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>3</v>
       </c>
@@ -1669,7 +1859,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>4</v>
       </c>
@@ -1683,7 +1873,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>5</v>
       </c>
@@ -1697,7 +1887,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>6</v>
       </c>
@@ -1711,7 +1901,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>7</v>
       </c>
@@ -1725,7 +1915,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>8</v>
       </c>
@@ -1739,7 +1929,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>9</v>
       </c>
@@ -1753,7 +1943,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>10</v>
       </c>
@@ -1767,7 +1957,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>11</v>
       </c>
@@ -1781,7 +1971,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>12</v>
       </c>
@@ -1795,7 +1985,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>1</v>
       </c>
@@ -1809,7 +1999,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>2</v>
       </c>
@@ -1823,7 +2013,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>3</v>
       </c>
@@ -1837,7 +2027,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>4</v>
       </c>
@@ -1851,7 +2041,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>5</v>
       </c>
@@ -1865,7 +2055,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>6</v>
       </c>
@@ -1879,7 +2069,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>7</v>
       </c>
@@ -1893,7 +2083,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>8</v>
       </c>
@@ -1907,7 +2097,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>9</v>
       </c>
@@ -1921,7 +2111,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>10</v>
       </c>
@@ -1935,7 +2125,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>11</v>
       </c>
@@ -1949,7 +2139,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>12</v>
       </c>
@@ -1963,7 +2153,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>1</v>
       </c>
@@ -1977,7 +2167,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>2</v>
       </c>
@@ -1991,7 +2181,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>3</v>
       </c>
@@ -2005,7 +2195,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>4</v>
       </c>
@@ -2019,7 +2209,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>5</v>
       </c>
@@ -2033,7 +2223,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>6</v>
       </c>
@@ -2047,7 +2237,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>7</v>
       </c>
@@ -2061,7 +2251,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>8</v>
       </c>
@@ -2075,7 +2265,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>9</v>
       </c>
@@ -2089,7 +2279,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>10</v>
       </c>
@@ -2103,7 +2293,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>11</v>
       </c>
@@ -2117,7 +2307,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>12</v>
       </c>
@@ -2131,7 +2321,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>1</v>
       </c>
@@ -2145,7 +2335,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>2</v>
       </c>
@@ -2159,7 +2349,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>3</v>
       </c>
@@ -2173,7 +2363,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>4</v>
       </c>
@@ -2187,7 +2377,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>5</v>
       </c>
@@ -2201,7 +2391,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>6</v>
       </c>
@@ -2215,7 +2405,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>7</v>
       </c>
@@ -2229,7 +2419,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>8</v>
       </c>
@@ -2243,7 +2433,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>9</v>
       </c>
@@ -2257,7 +2447,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>10</v>
       </c>
@@ -2271,7 +2461,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>11</v>
       </c>
@@ -2285,7 +2475,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>12</v>
       </c>
@@ -2299,7 +2489,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>1</v>
       </c>
@@ -2313,7 +2503,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>2</v>
       </c>
@@ -2327,7 +2517,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>3</v>
       </c>
@@ -2341,7 +2531,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>4</v>
       </c>
@@ -2355,7 +2545,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>5</v>
       </c>
@@ -2369,7 +2559,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>6</v>
       </c>
@@ -2383,7 +2573,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>7</v>
       </c>
@@ -2397,7 +2587,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>8</v>
       </c>
@@ -2411,7 +2601,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>9</v>
       </c>
@@ -2425,7 +2615,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>10</v>
       </c>
@@ -2439,7 +2629,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>11</v>
       </c>
@@ -2453,7 +2643,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>12</v>
       </c>
@@ -2467,7 +2657,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>1</v>
       </c>
@@ -2481,7 +2671,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>2</v>
       </c>
@@ -2495,7 +2685,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>3</v>
       </c>
@@ -2509,7 +2699,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>4</v>
       </c>
@@ -2523,7 +2713,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>5</v>
       </c>
@@ -2537,7 +2727,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>6</v>
       </c>
@@ -2551,7 +2741,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>7</v>
       </c>
@@ -2565,7 +2755,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>8</v>
       </c>
@@ -2579,7 +2769,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>9</v>
       </c>
@@ -2593,7 +2783,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>10</v>
       </c>
@@ -2607,7 +2797,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>11</v>
       </c>
@@ -2621,7 +2811,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>12</v>
       </c>
@@ -2635,7 +2825,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>1</v>
       </c>
@@ -2649,7 +2839,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>2</v>
       </c>
@@ -2663,7 +2853,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>3</v>
       </c>
@@ -2677,7 +2867,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>4</v>
       </c>
@@ -2691,7 +2881,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>5</v>
       </c>
@@ -2705,7 +2895,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>6</v>
       </c>
@@ -2719,7 +2909,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>7</v>
       </c>
@@ -2733,7 +2923,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>8</v>
       </c>
@@ -2747,7 +2937,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>9</v>
       </c>
@@ -2761,7 +2951,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>10</v>
       </c>
@@ -2775,7 +2965,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>11</v>
       </c>
@@ -2789,7 +2979,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>12</v>
       </c>
@@ -2803,7 +2993,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>1</v>
       </c>
@@ -2817,7 +3007,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>2</v>
       </c>
@@ -2831,7 +3021,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>3</v>
       </c>
@@ -2845,7 +3035,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>4</v>
       </c>
@@ -2859,7 +3049,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>5</v>
       </c>
@@ -2873,7 +3063,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>6</v>
       </c>
@@ -2887,7 +3077,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>7</v>
       </c>
@@ -2901,7 +3091,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>8</v>
       </c>
@@ -2915,7 +3105,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>9</v>
       </c>
@@ -2929,7 +3119,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>10</v>
       </c>
@@ -2943,7 +3133,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>11</v>
       </c>
@@ -2957,7 +3147,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>12</v>
       </c>
@@ -2971,7 +3161,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>1</v>
       </c>
@@ -2985,7 +3175,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>2</v>
       </c>
@@ -2999,7 +3189,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>3</v>
       </c>
@@ -3013,7 +3203,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>4</v>
       </c>
@@ -3027,7 +3217,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>5</v>
       </c>
@@ -3041,7 +3231,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>6</v>
       </c>
@@ -3055,7 +3245,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>7</v>
       </c>
@@ -3069,7 +3259,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>8</v>
       </c>
@@ -3083,7 +3273,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>9</v>
       </c>
@@ -3097,7 +3287,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>10</v>
       </c>
@@ -3111,7 +3301,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>11</v>
       </c>
@@ -3125,7 +3315,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>12</v>
       </c>
@@ -3139,7 +3329,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>1</v>
       </c>
@@ -3153,7 +3343,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>2</v>
       </c>
@@ -3167,7 +3357,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>3</v>
       </c>
@@ -3181,7 +3371,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>4</v>
       </c>
@@ -3195,7 +3385,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>5</v>
       </c>
@@ -3209,7 +3399,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>6</v>
       </c>
@@ -3223,7 +3413,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>7</v>
       </c>
@@ -3237,7 +3427,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>8</v>
       </c>
@@ -3251,7 +3441,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>9</v>
       </c>
@@ -3265,7 +3455,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>10</v>
       </c>
@@ -3279,7 +3469,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>11</v>
       </c>
@@ -3293,7 +3483,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>12</v>
       </c>
@@ -3307,7 +3497,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>1</v>
       </c>
@@ -3321,7 +3511,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>2</v>
       </c>
@@ -3335,7 +3525,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>3</v>
       </c>
@@ -3349,7 +3539,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>4</v>
       </c>
@@ -3363,7 +3553,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>5</v>
       </c>
@@ -3377,7 +3567,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>6</v>
       </c>
@@ -3391,7 +3581,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>7</v>
       </c>
@@ -3405,7 +3595,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>8</v>
       </c>
@@ -3419,7 +3609,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>9</v>
       </c>
@@ -3433,7 +3623,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>10</v>
       </c>
@@ -3447,7 +3637,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>11</v>
       </c>
@@ -3461,7 +3651,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>12</v>
       </c>
@@ -3475,7 +3665,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>1</v>
       </c>
@@ -3489,7 +3679,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>2</v>
       </c>
@@ -3503,7 +3693,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>3</v>
       </c>
@@ -3517,7 +3707,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>4</v>
       </c>
@@ -3531,7 +3721,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>5</v>
       </c>
@@ -3545,7 +3735,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>6</v>
       </c>
@@ -3559,7 +3749,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A152">
         <v>7</v>
       </c>
@@ -3573,7 +3763,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A153">
         <v>8</v>
       </c>
@@ -3587,7 +3777,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A154">
         <v>9</v>
       </c>
@@ -3601,7 +3791,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A155">
         <v>10</v>
       </c>
@@ -3615,7 +3805,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>11</v>
       </c>
@@ -3629,7 +3819,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A157">
         <v>12</v>
       </c>
@@ -3643,7 +3833,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A158">
         <v>1</v>
       </c>
@@ -3657,7 +3847,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A159">
         <v>2</v>
       </c>
@@ -3671,7 +3861,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A160">
         <v>3</v>
       </c>
@@ -3685,7 +3875,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>4</v>
       </c>
@@ -3699,7 +3889,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A162">
         <v>5</v>
       </c>
@@ -3713,7 +3903,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A163">
         <v>6</v>
       </c>
@@ -3727,7 +3917,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A164">
         <v>7</v>
       </c>
@@ -3741,7 +3931,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A165">
         <v>8</v>
       </c>
@@ -3755,7 +3945,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A166">
         <v>9</v>
       </c>
@@ -3769,7 +3959,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A167">
         <v>10</v>
       </c>
@@ -3783,7 +3973,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A168">
         <v>11</v>
       </c>
@@ -3797,7 +3987,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A169">
         <v>12</v>
       </c>
@@ -3811,7 +4001,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A170">
         <v>1</v>
       </c>
@@ -3825,7 +4015,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A171">
         <v>2</v>
       </c>
@@ -3839,7 +4029,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A172">
         <v>3</v>
       </c>
@@ -3853,7 +4043,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A173">
         <v>4</v>
       </c>
@@ -3867,7 +4057,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A174">
         <v>5</v>
       </c>
@@ -3881,7 +4071,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A175">
         <v>6</v>
       </c>
@@ -3895,7 +4085,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A176">
         <v>7</v>
       </c>
@@ -3909,7 +4099,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A177">
         <v>8</v>
       </c>
@@ -3923,7 +4113,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A178">
         <v>9</v>
       </c>
@@ -3937,7 +4127,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A179">
         <v>10</v>
       </c>
@@ -3951,7 +4141,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A180">
         <v>11</v>
       </c>
@@ -3965,7 +4155,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A181">
         <v>12</v>
       </c>
@@ -3979,7 +4169,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A182">
         <v>1</v>
       </c>
@@ -3993,7 +4183,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A183">
         <v>2</v>
       </c>
@@ -4007,7 +4197,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A184">
         <v>3</v>
       </c>
@@ -4021,7 +4211,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A185">
         <v>4</v>
       </c>
@@ -4035,7 +4225,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A186">
         <v>5</v>
       </c>
@@ -4049,7 +4239,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A187">
         <v>6</v>
       </c>
@@ -4063,7 +4253,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A188">
         <v>7</v>
       </c>
@@ -4077,7 +4267,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A189">
         <v>8</v>
       </c>
@@ -4091,7 +4281,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A190">
         <v>9</v>
       </c>
@@ -4105,7 +4295,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A191">
         <v>10</v>
       </c>
@@ -4119,7 +4309,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A192">
         <v>11</v>
       </c>
@@ -4133,7 +4323,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A193">
         <v>12</v>
       </c>
@@ -4147,7 +4337,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A194">
         <v>1</v>
       </c>
@@ -4161,7 +4351,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A195">
         <v>2</v>
       </c>
@@ -4175,7 +4365,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A196">
         <v>3</v>
       </c>
@@ -4189,7 +4379,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A197">
         <v>4</v>
       </c>
@@ -4203,7 +4393,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A198">
         <v>5</v>
       </c>
@@ -4217,7 +4407,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A199">
         <v>6</v>
       </c>
@@ -4231,7 +4421,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A200">
         <v>7</v>
       </c>
@@ -4245,7 +4435,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A201">
         <v>8</v>
       </c>
@@ -4259,7 +4449,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A202">
         <v>9</v>
       </c>
@@ -4273,7 +4463,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A203">
         <v>10</v>
       </c>
@@ -4287,7 +4477,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A204">
         <v>11</v>
       </c>
@@ -4301,7 +4491,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A205">
         <v>12</v>
       </c>
@@ -4315,7 +4505,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A206">
         <v>1</v>
       </c>
@@ -4329,7 +4519,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A207">
         <v>2</v>
       </c>
@@ -4343,7 +4533,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A208">
         <v>3</v>
       </c>
@@ -4357,7 +4547,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A209">
         <v>4</v>
       </c>
@@ -4371,7 +4561,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A210">
         <v>5</v>
       </c>
@@ -4385,7 +4575,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A211">
         <v>6</v>
       </c>
@@ -4399,7 +4589,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A212">
         <v>7</v>
       </c>
@@ -4413,7 +4603,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A213">
         <v>8</v>
       </c>
@@ -4427,7 +4617,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A214">
         <v>9</v>
       </c>
@@ -4441,7 +4631,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A215">
         <v>10</v>
       </c>
@@ -4455,7 +4645,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A216">
         <v>11</v>
       </c>
@@ -4469,7 +4659,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A217">
         <v>12</v>
       </c>
@@ -4483,7 +4673,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A218">
         <v>1</v>
       </c>
@@ -4497,7 +4687,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A219">
         <v>2</v>
       </c>
@@ -4511,7 +4701,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A220">
         <v>3</v>
       </c>
@@ -4525,7 +4715,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A221">
         <v>4</v>
       </c>
@@ -4539,7 +4729,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A222">
         <v>5</v>
       </c>
@@ -4553,7 +4743,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A223">
         <v>6</v>
       </c>
@@ -4567,7 +4757,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A224">
         <v>7</v>
       </c>
@@ -4581,7 +4771,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A225">
         <v>8</v>
       </c>
@@ -4595,7 +4785,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A226">
         <v>9</v>
       </c>
@@ -4609,7 +4799,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A227">
         <v>10</v>
       </c>
@@ -4623,7 +4813,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A228">
         <v>11</v>
       </c>
@@ -4637,7 +4827,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="229" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A229">
         <v>12</v>
       </c>
@@ -4651,7 +4841,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A230">
         <v>1</v>
       </c>
@@ -4665,7 +4855,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="231" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A231">
         <v>2</v>
       </c>
@@ -4679,7 +4869,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A232">
         <v>3</v>
       </c>
@@ -4693,7 +4883,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A233">
         <v>4</v>
       </c>
@@ -4707,7 +4897,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A234">
         <v>5</v>
       </c>
@@ -4721,7 +4911,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="235" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A235">
         <v>6</v>
       </c>
@@ -4735,7 +4925,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="236" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A236">
         <v>7</v>
       </c>
@@ -4749,7 +4939,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="237" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A237">
         <v>8</v>
       </c>
@@ -4763,7 +4953,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="238" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A238">
         <v>9</v>
       </c>
@@ -4777,7 +4967,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="239" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A239">
         <v>10</v>
       </c>
@@ -4791,7 +4981,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="240" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A240">
         <v>11</v>
       </c>
@@ -4805,7 +4995,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="241" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A241">
         <v>12</v>
       </c>
@@ -4819,7 +5009,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A242">
         <v>1</v>
       </c>
@@ -4833,7 +5023,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="243" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A243">
         <v>2</v>
       </c>
@@ -4847,7 +5037,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="244" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A244">
         <v>3</v>
       </c>
@@ -4861,7 +5051,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="245" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A245">
         <v>4</v>
       </c>
@@ -4875,7 +5065,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="246" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A246">
         <v>5</v>
       </c>
@@ -4889,7 +5079,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="247" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A247">
         <v>6</v>
       </c>
@@ -4903,7 +5093,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="248" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A248">
         <v>7</v>
       </c>
@@ -4917,7 +5107,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="249" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A249">
         <v>8</v>
       </c>
@@ -4931,7 +5121,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="250" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A250">
         <v>9</v>
       </c>
@@ -4945,7 +5135,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="251" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A251">
         <v>10</v>
       </c>
@@ -4959,7 +5149,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="252" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A252">
         <v>11</v>
       </c>
@@ -4973,7 +5163,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="253" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A253">
         <v>12</v>
       </c>
@@ -4987,7 +5177,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="254" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A254">
         <v>1</v>
       </c>
@@ -5001,7 +5191,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="255" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A255">
         <v>2</v>
       </c>
@@ -5015,7 +5205,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="256" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A256">
         <v>3</v>
       </c>
@@ -5029,7 +5219,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="257" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A257">
         <v>4</v>
       </c>
@@ -5043,7 +5233,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="258" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A258">
         <v>5</v>
       </c>
@@ -5057,7 +5247,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="259" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A259">
         <v>6</v>
       </c>
@@ -5071,7 +5261,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="260" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A260">
         <v>7</v>
       </c>
@@ -5085,7 +5275,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="261" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A261">
         <v>8</v>
       </c>
@@ -5099,7 +5289,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="262" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A262">
         <v>9</v>
       </c>
@@ -5113,7 +5303,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="263" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A263">
         <v>10</v>
       </c>
@@ -5127,7 +5317,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="264" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A264">
         <v>11</v>
       </c>
@@ -5141,7 +5331,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="265" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A265">
         <v>12</v>
       </c>
@@ -5155,7 +5345,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="266" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A266">
         <v>1</v>
       </c>
@@ -5169,7 +5359,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="267" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A267">
         <v>2</v>
       </c>
@@ -5183,7 +5373,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="268" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A268">
         <v>3</v>
       </c>
@@ -5197,7 +5387,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="269" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A269">
         <v>4</v>
       </c>
@@ -5211,7 +5401,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="270" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A270">
         <v>5</v>
       </c>
@@ -5225,7 +5415,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="271" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A271">
         <v>6</v>
       </c>
@@ -5239,7 +5429,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="272" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A272">
         <v>7</v>
       </c>
@@ -5253,7 +5443,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="273" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A273">
         <v>8</v>
       </c>
@@ -5267,7 +5457,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="274" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A274">
         <v>9</v>
       </c>
@@ -5281,7 +5471,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="275" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A275">
         <v>10</v>
       </c>
@@ -5295,7 +5485,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="276" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A276">
         <v>11</v>
       </c>
@@ -5309,7 +5499,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="277" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A277">
         <v>12</v>
       </c>
@@ -5323,7 +5513,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="278" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A278">
         <v>1</v>
       </c>
@@ -5337,7 +5527,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="279" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A279">
         <v>2</v>
       </c>
@@ -5351,7 +5541,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="280" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A280">
         <v>3</v>
       </c>
@@ -5365,7 +5555,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="281" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A281">
         <v>4</v>
       </c>
@@ -5379,7 +5569,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="282" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A282">
         <v>5</v>
       </c>
@@ -5393,7 +5583,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="283" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A283">
         <v>6</v>
       </c>
@@ -5407,7 +5597,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="284" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A284">
         <v>7</v>
       </c>
@@ -5421,7 +5611,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="285" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A285">
         <v>8</v>
       </c>
@@ -5435,7 +5625,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="286" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A286">
         <v>9</v>
       </c>
@@ -5449,7 +5639,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="287" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A287">
         <v>10</v>
       </c>
@@ -5463,7 +5653,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="288" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A288">
         <v>11</v>
       </c>
@@ -5477,7 +5667,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="289" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A289">
         <v>12</v>
       </c>
@@ -5491,7 +5681,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="290" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A290">
         <v>1</v>
       </c>
@@ -5505,7 +5695,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="291" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A291">
         <v>2</v>
       </c>
@@ -5519,7 +5709,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="292" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A292">
         <v>3</v>
       </c>
@@ -5533,7 +5723,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="293" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A293">
         <v>4</v>
       </c>
@@ -5547,7 +5737,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="294" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A294">
         <v>5</v>
       </c>
@@ -5561,7 +5751,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="295" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A295">
         <v>6</v>
       </c>
@@ -5575,7 +5765,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="296" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A296">
         <v>7</v>
       </c>
@@ -5589,7 +5779,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="297" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A297">
         <v>8</v>
       </c>
@@ -5603,7 +5793,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="298" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A298">
         <v>9</v>
       </c>
@@ -5617,7 +5807,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="299" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A299">
         <v>10</v>
       </c>
@@ -5631,7 +5821,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="300" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A300">
         <v>11</v>
       </c>
@@ -5645,7 +5835,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="301" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A301">
         <v>12</v>
       </c>
@@ -5659,7 +5849,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="302" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A302">
         <v>1</v>
       </c>
@@ -5673,7 +5863,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="303" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A303">
         <v>2</v>
       </c>
@@ -5687,7 +5877,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="304" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A304">
         <v>3</v>
       </c>
@@ -5701,7 +5891,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="305" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A305">
         <v>4</v>
       </c>
@@ -5715,7 +5905,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="306" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A306">
         <v>5</v>
       </c>
@@ -5729,7 +5919,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="307" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A307">
         <v>6</v>
       </c>
@@ -5743,7 +5933,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="308" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A308">
         <v>7</v>
       </c>
@@ -5757,7 +5947,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="309" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A309">
         <v>8</v>
       </c>
@@ -5771,7 +5961,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="310" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A310">
         <v>9</v>
       </c>
@@ -5785,7 +5975,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="311" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A311">
         <v>10</v>
       </c>
@@ -5799,7 +5989,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="312" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A312">
         <v>11</v>
       </c>
@@ -5813,7 +6003,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="313" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A313">
         <v>12</v>
       </c>
@@ -5827,7 +6017,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="314" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A314">
         <v>1</v>
       </c>
@@ -5841,7 +6031,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="315" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A315">
         <v>2</v>
       </c>
@@ -5855,7 +6045,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="316" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A316">
         <v>3</v>
       </c>
@@ -5869,7 +6059,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="317" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A317">
         <v>4</v>
       </c>
@@ -5883,7 +6073,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="318" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A318">
         <v>5</v>
       </c>
@@ -5897,7 +6087,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="319" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A319">
         <v>6</v>
       </c>
@@ -5911,7 +6101,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="320" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A320">
         <v>7</v>
       </c>
@@ -5925,7 +6115,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="321" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A321">
         <v>8</v>
       </c>
@@ -5939,7 +6129,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="322" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A322">
         <v>9</v>
       </c>
@@ -5953,7 +6143,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="323" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A323">
         <v>10</v>
       </c>
@@ -5967,7 +6157,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="324" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A324">
         <v>11</v>
       </c>
@@ -5981,7 +6171,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="325" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A325">
         <v>12</v>
       </c>
@@ -6002,25 +6192,25 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71493739-45C2-4A8D-9266-24BB3FC8F4DB}">
-  <dimension ref="A1:O18"/>
+  <dimension ref="A1:T18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="2" max="2" width="14.44140625" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" customWidth="1"/>
-    <col min="7" max="7" width="18.28515625" customWidth="1"/>
+    <col min="6" max="6" width="17.44140625" customWidth="1"/>
+    <col min="7" max="7" width="18.33203125" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
-    <col min="9" max="9" width="19.28515625" customWidth="1"/>
-    <col min="10" max="10" width="21.85546875" customWidth="1"/>
-    <col min="14" max="14" width="20.140625" customWidth="1"/>
+    <col min="9" max="9" width="19.33203125" customWidth="1"/>
+    <col min="10" max="10" width="21.88671875" customWidth="1"/>
+    <col min="14" max="14" width="20.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>18</v>
       </c>
@@ -6066,8 +6256,23 @@
       <c r="O1" s="6" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P1" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q1" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="R1" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="S1" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="T1" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>27</v>
       </c>
@@ -6113,8 +6318,23 @@
       <c r="O2" s="7">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P2" s="7">
+        <v>20</v>
+      </c>
+      <c r="Q2" s="7">
+        <v>25</v>
+      </c>
+      <c r="R2" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="S2" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="T2" s="7">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>31</v>
       </c>
@@ -6160,50 +6380,67 @@
       <c r="O3" s="7">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P3" s="7">
+        <v>20</v>
+      </c>
+      <c r="Q3" s="7">
+        <v>25</v>
+      </c>
+      <c r="R3" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="S3" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="T3" s="7">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" s="5"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" s="5"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" s="5"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" s="5"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" s="5"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" s="5"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14" s="5"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" s="5"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="5"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" s="5"/>
     </row>
   </sheetData>
@@ -6220,9 +6457,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -6235,7 +6472,7 @@
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2024</v>
       </c>
@@ -6246,7 +6483,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2025</v>
       </c>
@@ -6257,7 +6494,7 @@
         <v>2.2200000000000001E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2026</v>
       </c>
@@ -6268,7 +6505,7 @@
         <v>2.4400000000000002E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2027</v>
       </c>
@@ -6279,7 +6516,7 @@
         <v>2.6599999999999999E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2028</v>
       </c>
@@ -6290,7 +6527,7 @@
         <v>2.8799999999999999E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2029</v>
       </c>
@@ -6301,7 +6538,7 @@
         <v>3.1E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2030</v>
       </c>
@@ -6312,7 +6549,7 @@
         <v>3.32E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2031</v>
       </c>
@@ -6323,7 +6560,7 @@
         <v>3.5400000000000001E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2032</v>
       </c>
@@ -6334,7 +6571,7 @@
         <v>3.7600000000000001E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2033</v>
       </c>
@@ -6345,7 +6582,7 @@
         <v>3.9800000000000002E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2034</v>
       </c>
@@ -6356,7 +6593,7 @@
         <v>3.9800000000000002E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2035</v>
       </c>
@@ -6367,7 +6604,7 @@
         <v>4.2000000000000003E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2036</v>
       </c>
@@ -6378,7 +6615,7 @@
         <v>4.4200000000000003E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2037</v>
       </c>
@@ -6389,7 +6626,7 @@
         <v>4.6399999999999997E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2038</v>
       </c>
@@ -6400,7 +6637,7 @@
         <v>4.8599999999999997E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2039</v>
       </c>
@@ -6411,7 +6648,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2040</v>
       </c>
@@ -6422,7 +6659,7 @@
         <v>5.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2041</v>
       </c>
@@ -6433,7 +6670,7 @@
         <v>5.5199999999999999E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2042</v>
       </c>
@@ -6444,7 +6681,7 @@
         <v>5.74E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>2043</v>
       </c>
@@ -6455,7 +6692,7 @@
         <v>5.96E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>2044</v>
       </c>
@@ -6466,7 +6703,7 @@
         <v>6.1800000000000001E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>2045</v>
       </c>
@@ -6477,7 +6714,7 @@
         <v>6.4000000000000001E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>2046</v>
       </c>
@@ -6488,7 +6725,7 @@
         <v>6.6199999999999995E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>2047</v>
       </c>
@@ -6499,7 +6736,7 @@
         <v>6.8400000000000002E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>2048</v>
       </c>
@@ -6510,7 +6747,7 @@
         <v>7.0599999999999996E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>2049</v>
       </c>
@@ -6521,7 +6758,7 @@
         <v>7.2800000000000004E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>2050</v>
       </c>
@@ -6545,9 +6782,9 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -6560,7 +6797,7 @@
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2024</v>
       </c>
@@ -6571,7 +6808,7 @@
         <v>26229.707720000002</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2025</v>
       </c>
@@ -6582,7 +6819,7 @@
         <v>26589.174669999997</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2026</v>
       </c>
@@ -6593,7 +6830,7 @@
         <v>60431.69513</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2027</v>
       </c>
@@ -6604,7 +6841,7 @@
         <v>95314.195130000007</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2028</v>
       </c>
@@ -6615,7 +6852,7 @@
         <v>130196.6951</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2029</v>
       </c>
@@ -6626,7 +6863,7 @@
         <v>165780.465</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2030</v>
       </c>
@@ -6637,7 +6874,7 @@
         <v>179750.54879999999</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2031</v>
       </c>
@@ -6648,7 +6885,7 @@
         <v>195610.7611</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2032</v>
       </c>
@@ -6659,7 +6896,7 @@
         <v>196499.72339999999</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2033</v>
       </c>
@@ -6670,7 +6907,7 @@
         <v>198853.9976</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2034</v>
       </c>
@@ -6681,7 +6918,7 @@
         <v>202089.00579999998</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2035</v>
       </c>
@@ -6692,7 +6929,7 @@
         <v>164077.8836</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2036</v>
       </c>
@@ -6703,7 +6940,7 @@
         <v>126654.49769999999</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2037</v>
       </c>
@@ -6714,7 +6951,7 @@
         <v>90701.344779999999</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2038</v>
       </c>
@@ -6725,7 +6962,7 @@
         <v>57298.538379999998</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2039</v>
       </c>
@@ -6736,7 +6973,7 @@
         <v>40938.322699999997</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2040</v>
       </c>
@@ -6747,7 +6984,7 @@
         <v>30788.296410000003</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2041</v>
       </c>
@@ -6758,7 +6995,7 @@
         <v>28368.054080000002</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2042</v>
       </c>
@@ -6769,7 +7006,7 @@
         <v>31250.81408</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>2043</v>
       </c>
@@ -6780,7 +7017,7 @@
         <v>34011.350160000002</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>2044</v>
       </c>
@@ -6791,7 +7028,7 @@
         <v>35066.675019999995</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>2045</v>
       </c>
@@ -6802,7 +7039,7 @@
         <v>33453.543590000001</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>2046</v>
       </c>
@@ -6813,7 +7050,7 @@
         <v>25310.301890000002</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>2047</v>
       </c>
@@ -6824,7 +7061,7 @@
         <v>11877.08452</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>2048</v>
       </c>
@@ -6835,7 +7072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>2049</v>
       </c>
@@ -6846,7 +7083,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>2050</v>
       </c>
@@ -6870,9 +7107,9 @@
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -6885,7 +7122,7 @@
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2024</v>
       </c>
@@ -6896,7 +7133,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2025</v>
       </c>
@@ -6907,7 +7144,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2026</v>
       </c>
@@ -6918,7 +7155,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2027</v>
       </c>
@@ -6929,7 +7166,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2028</v>
       </c>
@@ -6940,7 +7177,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2029</v>
       </c>
@@ -6951,7 +7188,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2030</v>
       </c>
@@ -6962,7 +7199,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2031</v>
       </c>
@@ -6973,7 +7210,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2032</v>
       </c>
@@ -6984,7 +7221,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2033</v>
       </c>
@@ -6995,7 +7232,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2034</v>
       </c>
@@ -7006,7 +7243,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2035</v>
       </c>
@@ -7017,7 +7254,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2036</v>
       </c>
@@ -7028,7 +7265,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2037</v>
       </c>
@@ -7039,7 +7276,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2038</v>
       </c>
@@ -7050,7 +7287,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2039</v>
       </c>
@@ -7061,7 +7298,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2040</v>
       </c>
@@ -7072,7 +7309,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2041</v>
       </c>
@@ -7083,7 +7320,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2042</v>
       </c>
@@ -7094,7 +7331,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>2043</v>
       </c>
@@ -7105,7 +7342,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>2044</v>
       </c>
@@ -7116,7 +7353,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>2045</v>
       </c>
@@ -7127,7 +7364,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>2046</v>
       </c>
@@ -7138,7 +7375,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>2047</v>
       </c>
@@ -7149,7 +7386,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>2048</v>
       </c>
@@ -7160,7 +7397,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>2049</v>
       </c>
@@ -7171,7 +7408,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>2050</v>
       </c>

</xml_diff>

<commit_message>
Implemented rolling horizon. Not working at all :)
</commit_message>
<xml_diff>
--- a/Input_urbsextensionv1.xlsx
+++ b/Input_urbsextensionv1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxoi\GitHub\urbs-extension\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5CDF984-1904-4865-89C0-861161723B77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AD04B97-CDB3-4A5F-B0D1-09AA9779FDF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="67080" yWindow="-1935" windowWidth="29040" windowHeight="17520" activeTab="7" xr2:uid="{81864710-3A67-40FC-ABA1-4EF02E4F8A12}"/>
+    <workbookView xWindow="28680" yWindow="-5445" windowWidth="38640" windowHeight="21120" activeTab="7" xr2:uid="{81864710-3A67-40FC-ABA1-4EF02E4F8A12}"/>
   </bookViews>
   <sheets>
     <sheet name="Base" sheetId="10" r:id="rId1"/>
@@ -739,7 +739,7 @@
   <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7527,8 +7527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71493739-45C2-4A8D-9266-24BB3FC8F4DB}">
   <dimension ref="A1:T18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="W7" sqref="W7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7541,6 +7541,7 @@
     <col min="9" max="9" width="19.33203125" customWidth="1"/>
     <col min="10" max="10" width="21.88671875" customWidth="1"/>
     <col min="14" max="14" width="20.109375" customWidth="1"/>
+    <col min="20" max="20" width="20.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.3">
@@ -7696,7 +7697,7 @@
         <v>7.2700000000000001E-2</v>
       </c>
       <c r="J3" s="7">
-        <v>0.38879999999999998</v>
+        <v>7.2700000000000001E-2</v>
       </c>
       <c r="K3" s="7">
         <v>0.8</v>
@@ -7720,7 +7721,7 @@
         <v>10000</v>
       </c>
       <c r="R3" s="7">
-        <v>0.85</v>
+        <v>0.7</v>
       </c>
       <c r="S3" s="7">
         <v>0.2</v>
@@ -7758,7 +7759,7 @@
         <v>7.2700000000000001E-2</v>
       </c>
       <c r="J4" s="7">
-        <v>0.38879999999999998</v>
+        <v>7.2700000000000001E-2</v>
       </c>
       <c r="K4" s="7">
         <v>0.8</v>
@@ -7782,7 +7783,7 @@
         <v>10000</v>
       </c>
       <c r="R4" s="7">
-        <v>0.85</v>
+        <v>0.7</v>
       </c>
       <c r="S4" s="7">
         <v>0.2</v>
@@ -8660,7 +8661,7 @@
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18:C28"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8685,13 +8686,13 @@
         <v>2024</v>
       </c>
       <c r="B2" s="4">
-        <v>93020</v>
+        <v>150000</v>
       </c>
       <c r="C2">
-        <v>25000</v>
+        <v>13333</v>
       </c>
       <c r="D2">
-        <v>50000</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -8702,10 +8703,10 @@
         <v>93020</v>
       </c>
       <c r="C3">
-        <v>25000</v>
+        <v>13333</v>
       </c>
       <c r="D3">
-        <v>50000</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -8716,10 +8717,10 @@
         <v>93020</v>
       </c>
       <c r="C4">
-        <v>25000</v>
+        <v>13333</v>
       </c>
       <c r="D4">
-        <v>50000</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -8730,10 +8731,10 @@
         <v>93020</v>
       </c>
       <c r="C5">
-        <v>25000</v>
+        <v>13333</v>
       </c>
       <c r="D5">
-        <v>50000</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -8744,10 +8745,10 @@
         <v>93020</v>
       </c>
       <c r="C6">
-        <v>25000</v>
+        <v>13333</v>
       </c>
       <c r="D6">
-        <v>50000</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -8758,10 +8759,10 @@
         <v>93020</v>
       </c>
       <c r="C7">
-        <v>25000</v>
+        <v>13333</v>
       </c>
       <c r="D7">
-        <v>50000</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -8772,10 +8773,10 @@
         <v>93020</v>
       </c>
       <c r="C8">
+        <v>20000</v>
+      </c>
+      <c r="D8">
         <v>30000</v>
-      </c>
-      <c r="D8">
-        <v>50000</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -8786,10 +8787,10 @@
         <v>61911.5</v>
       </c>
       <c r="C9">
+        <v>20000</v>
+      </c>
+      <c r="D9">
         <v>30000</v>
-      </c>
-      <c r="D9">
-        <v>50000</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -8800,10 +8801,10 @@
         <v>61911.5</v>
       </c>
       <c r="C10">
+        <v>20000</v>
+      </c>
+      <c r="D10">
         <v>30000</v>
-      </c>
-      <c r="D10">
-        <v>50000</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -8814,10 +8815,10 @@
         <v>61911.5</v>
       </c>
       <c r="C11">
+        <v>20000</v>
+      </c>
+      <c r="D11">
         <v>30000</v>
-      </c>
-      <c r="D11">
-        <v>50000</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -8828,10 +8829,10 @@
         <v>61911.5</v>
       </c>
       <c r="C12">
+        <v>20000</v>
+      </c>
+      <c r="D12">
         <v>30000</v>
-      </c>
-      <c r="D12">
-        <v>50000</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -8842,10 +8843,10 @@
         <v>61911.5</v>
       </c>
       <c r="C13">
+        <v>20000</v>
+      </c>
+      <c r="D13">
         <v>30000</v>
-      </c>
-      <c r="D13">
-        <v>50000</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -8856,10 +8857,10 @@
         <v>61911.5</v>
       </c>
       <c r="C14">
+        <v>20000</v>
+      </c>
+      <c r="D14">
         <v>30000</v>
-      </c>
-      <c r="D14">
-        <v>50000</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -8870,10 +8871,10 @@
         <v>61911.5</v>
       </c>
       <c r="C15">
+        <v>20000</v>
+      </c>
+      <c r="D15">
         <v>30000</v>
-      </c>
-      <c r="D15">
-        <v>50000</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -8884,10 +8885,10 @@
         <v>61911.5</v>
       </c>
       <c r="C16">
+        <v>20000</v>
+      </c>
+      <c r="D16">
         <v>30000</v>
-      </c>
-      <c r="D16">
-        <v>50000</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -8898,10 +8899,10 @@
         <v>61911.5</v>
       </c>
       <c r="C17">
+        <v>20000</v>
+      </c>
+      <c r="D17">
         <v>30000</v>
-      </c>
-      <c r="D17">
-        <v>50000</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -8912,10 +8913,10 @@
         <v>61911.5</v>
       </c>
       <c r="C18">
-        <v>40000</v>
+        <v>20000</v>
       </c>
       <c r="D18">
-        <v>35000</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -8926,10 +8927,10 @@
         <v>57655.199999999997</v>
       </c>
       <c r="C19">
-        <v>40000</v>
+        <v>20000</v>
       </c>
       <c r="D19">
-        <v>35000</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -8940,10 +8941,10 @@
         <v>57655.199999999997</v>
       </c>
       <c r="C20">
-        <v>40000</v>
+        <v>20000</v>
       </c>
       <c r="D20">
-        <v>35000</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -8954,10 +8955,10 @@
         <v>57655.199999999997</v>
       </c>
       <c r="C21">
-        <v>40000</v>
+        <v>20000</v>
       </c>
       <c r="D21">
-        <v>35000</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -8968,10 +8969,10 @@
         <v>57655.199999999997</v>
       </c>
       <c r="C22">
-        <v>40000</v>
+        <v>20000</v>
       </c>
       <c r="D22">
-        <v>35000</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -8982,10 +8983,10 @@
         <v>57655.199999999997</v>
       </c>
       <c r="C23">
-        <v>40000</v>
+        <v>20000</v>
       </c>
       <c r="D23">
-        <v>35000</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -8996,10 +8997,10 @@
         <v>57655.199999999997</v>
       </c>
       <c r="C24">
-        <v>40000</v>
+        <v>20000</v>
       </c>
       <c r="D24">
-        <v>35000</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -9010,10 +9011,10 @@
         <v>57655.199999999997</v>
       </c>
       <c r="C25">
-        <v>40000</v>
+        <v>20000</v>
       </c>
       <c r="D25">
-        <v>35000</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -9024,10 +9025,10 @@
         <v>57655.199999999997</v>
       </c>
       <c r="C26">
-        <v>40000</v>
+        <v>20000</v>
       </c>
       <c r="D26">
-        <v>9999999</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
@@ -9038,10 +9039,10 @@
         <v>57655.199999999997</v>
       </c>
       <c r="C27">
-        <v>40000</v>
+        <v>20000</v>
       </c>
       <c r="D27">
-        <v>9999999</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
@@ -9052,10 +9053,10 @@
         <v>57655.199999999997</v>
       </c>
       <c r="C28">
-        <v>40000</v>
+        <v>20000</v>
       </c>
       <c r="D28">
-        <v>9999999</v>
+        <v>30000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
IMPLEMENTED FEEDBACK - ROLLLING HORIZON - TODO CHECK IF LR WORK PROPERLY
</commit_message>
<xml_diff>
--- a/Input_urbsextensionv1.xlsx
+++ b/Input_urbsextensionv1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxoi\GitHub\urbs-extension\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AD04B97-CDB3-4A5F-B0D1-09AA9779FDF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D88DD8F-3C38-47CA-A616-17733F889E38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-5445" windowWidth="38640" windowHeight="21120" activeTab="7" xr2:uid="{81864710-3A67-40FC-ABA1-4EF02E4F8A12}"/>
+    <workbookView xWindow="28680" yWindow="-5445" windowWidth="38640" windowHeight="21120" activeTab="4" xr2:uid="{81864710-3A67-40FC-ABA1-4EF02E4F8A12}"/>
   </bookViews>
   <sheets>
     <sheet name="Base" sheetId="10" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="48">
   <si>
     <t>Value</t>
   </si>
@@ -184,6 +184,9 @@
   </si>
   <si>
     <t>recycling_EU27_windon</t>
+  </si>
+  <si>
+    <t>Initial_secondary_cap</t>
   </si>
 </sst>
 </file>
@@ -331,13 +334,12 @@
     </xf>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -739,7 +741,7 @@
   <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -747,6 +749,7 @@
     <col min="2" max="2" width="13.6640625" customWidth="1"/>
     <col min="3" max="3" width="26.6640625" customWidth="1"/>
     <col min="4" max="4" width="37.33203125" customWidth="1"/>
+    <col min="5" max="5" width="29.88671875" customWidth="1"/>
     <col min="6" max="6" width="39.88671875" customWidth="1"/>
     <col min="7" max="7" width="21.44140625" customWidth="1"/>
     <col min="9" max="9" width="22.5546875" customWidth="1"/>
@@ -820,7 +823,7 @@
       <c r="H2">
         <v>9999999</v>
       </c>
-      <c r="I2" s="7">
+      <c r="I2" s="6">
         <v>11000</v>
       </c>
       <c r="J2">
@@ -832,7 +835,7 @@
       <c r="L2">
         <v>9999999</v>
       </c>
-      <c r="M2" s="7">
+      <c r="M2" s="6">
         <v>11000</v>
       </c>
     </row>
@@ -861,7 +864,7 @@
       <c r="H3">
         <v>9999999</v>
       </c>
-      <c r="I3" s="7">
+      <c r="I3" s="6">
         <v>11000</v>
       </c>
       <c r="J3">
@@ -873,7 +876,7 @@
       <c r="L3">
         <v>9999999</v>
       </c>
-      <c r="M3" s="7">
+      <c r="M3" s="6">
         <v>11000</v>
       </c>
     </row>
@@ -902,7 +905,7 @@
       <c r="H4">
         <v>9999999</v>
       </c>
-      <c r="I4" s="7">
+      <c r="I4" s="6">
         <v>11000</v>
       </c>
       <c r="J4">
@@ -914,7 +917,7 @@
       <c r="L4">
         <v>9999999</v>
       </c>
-      <c r="M4" s="7">
+      <c r="M4" s="6">
         <v>11000</v>
       </c>
     </row>
@@ -943,7 +946,7 @@
       <c r="H5">
         <v>9999999</v>
       </c>
-      <c r="I5" s="7">
+      <c r="I5" s="6">
         <v>11000</v>
       </c>
       <c r="J5">
@@ -955,7 +958,7 @@
       <c r="L5">
         <v>9999999</v>
       </c>
-      <c r="M5" s="7">
+      <c r="M5" s="6">
         <v>11000</v>
       </c>
     </row>
@@ -984,7 +987,7 @@
       <c r="H6">
         <v>9999999</v>
       </c>
-      <c r="I6" s="7">
+      <c r="I6" s="6">
         <v>11000</v>
       </c>
       <c r="J6">
@@ -996,7 +999,7 @@
       <c r="L6">
         <v>9999999</v>
       </c>
-      <c r="M6" s="7">
+      <c r="M6" s="6">
         <v>11000</v>
       </c>
     </row>
@@ -1025,7 +1028,7 @@
       <c r="H7">
         <v>9999999</v>
       </c>
-      <c r="I7" s="7">
+      <c r="I7" s="6">
         <v>11000</v>
       </c>
       <c r="J7">
@@ -1037,7 +1040,7 @@
       <c r="L7">
         <v>9999999</v>
       </c>
-      <c r="M7" s="7">
+      <c r="M7" s="6">
         <v>11000</v>
       </c>
     </row>
@@ -1066,7 +1069,7 @@
       <c r="H8">
         <v>9999999</v>
       </c>
-      <c r="I8" s="7">
+      <c r="I8" s="6">
         <v>11000</v>
       </c>
       <c r="J8">
@@ -1078,7 +1081,7 @@
       <c r="L8">
         <v>9999999</v>
       </c>
-      <c r="M8" s="7">
+      <c r="M8" s="6">
         <v>11000</v>
       </c>
     </row>
@@ -1107,7 +1110,7 @@
       <c r="H9">
         <v>9999999</v>
       </c>
-      <c r="I9" s="7">
+      <c r="I9" s="6">
         <v>11000</v>
       </c>
       <c r="J9">
@@ -1119,7 +1122,7 @@
       <c r="L9">
         <v>9999999</v>
       </c>
-      <c r="M9" s="7">
+      <c r="M9" s="6">
         <v>11000</v>
       </c>
     </row>
@@ -1148,7 +1151,7 @@
       <c r="H10">
         <v>9999999</v>
       </c>
-      <c r="I10" s="7">
+      <c r="I10" s="6">
         <v>11000</v>
       </c>
       <c r="J10">
@@ -1160,7 +1163,7 @@
       <c r="L10">
         <v>9999999</v>
       </c>
-      <c r="M10" s="7">
+      <c r="M10" s="6">
         <v>11000</v>
       </c>
     </row>
@@ -1189,7 +1192,7 @@
       <c r="H11">
         <v>9999999</v>
       </c>
-      <c r="I11" s="7">
+      <c r="I11" s="6">
         <v>11000</v>
       </c>
       <c r="J11">
@@ -1201,7 +1204,7 @@
       <c r="L11">
         <v>9999999</v>
       </c>
-      <c r="M11" s="7">
+      <c r="M11" s="6">
         <v>11000</v>
       </c>
     </row>
@@ -1230,7 +1233,7 @@
       <c r="H12">
         <v>9999999</v>
       </c>
-      <c r="I12" s="7">
+      <c r="I12" s="6">
         <v>11000</v>
       </c>
       <c r="J12">
@@ -1242,7 +1245,7 @@
       <c r="L12">
         <v>9999999</v>
       </c>
-      <c r="M12" s="7">
+      <c r="M12" s="6">
         <v>11000</v>
       </c>
     </row>
@@ -1271,7 +1274,7 @@
       <c r="H13">
         <v>9999999</v>
       </c>
-      <c r="I13" s="7">
+      <c r="I13" s="6">
         <v>11000</v>
       </c>
       <c r="J13">
@@ -1283,7 +1286,7 @@
       <c r="L13">
         <v>9999999</v>
       </c>
-      <c r="M13" s="7">
+      <c r="M13" s="6">
         <v>11000</v>
       </c>
     </row>
@@ -1312,7 +1315,7 @@
       <c r="H14">
         <v>9999999</v>
       </c>
-      <c r="I14" s="7">
+      <c r="I14" s="6">
         <v>11000</v>
       </c>
       <c r="J14">
@@ -1324,7 +1327,7 @@
       <c r="L14">
         <v>9999999</v>
       </c>
-      <c r="M14" s="7">
+      <c r="M14" s="6">
         <v>11000</v>
       </c>
     </row>
@@ -1353,7 +1356,7 @@
       <c r="H15">
         <v>9999999</v>
       </c>
-      <c r="I15" s="7">
+      <c r="I15" s="6">
         <v>11000</v>
       </c>
       <c r="J15">
@@ -1365,7 +1368,7 @@
       <c r="L15">
         <v>9999999</v>
       </c>
-      <c r="M15" s="7">
+      <c r="M15" s="6">
         <v>11000</v>
       </c>
     </row>
@@ -1394,7 +1397,7 @@
       <c r="H16">
         <v>9999999</v>
       </c>
-      <c r="I16" s="7">
+      <c r="I16" s="6">
         <v>11000</v>
       </c>
       <c r="J16">
@@ -1406,7 +1409,7 @@
       <c r="L16">
         <v>9999999</v>
       </c>
-      <c r="M16" s="7">
+      <c r="M16" s="6">
         <v>11000</v>
       </c>
     </row>
@@ -1435,7 +1438,7 @@
       <c r="H17">
         <v>9999999</v>
       </c>
-      <c r="I17" s="7">
+      <c r="I17" s="6">
         <v>11000</v>
       </c>
       <c r="J17">
@@ -1447,7 +1450,7 @@
       <c r="L17">
         <v>9999999</v>
       </c>
-      <c r="M17" s="7">
+      <c r="M17" s="6">
         <v>11000</v>
       </c>
     </row>
@@ -1476,7 +1479,7 @@
       <c r="H18">
         <v>9999999</v>
       </c>
-      <c r="I18" s="7">
+      <c r="I18" s="6">
         <v>11000</v>
       </c>
       <c r="J18">
@@ -1488,7 +1491,7 @@
       <c r="L18">
         <v>9999999</v>
       </c>
-      <c r="M18" s="7">
+      <c r="M18" s="6">
         <v>11000</v>
       </c>
     </row>
@@ -1517,7 +1520,7 @@
       <c r="H19">
         <v>9999999</v>
       </c>
-      <c r="I19" s="7">
+      <c r="I19" s="6">
         <v>11000</v>
       </c>
       <c r="J19">
@@ -1529,7 +1532,7 @@
       <c r="L19">
         <v>9999999</v>
       </c>
-      <c r="M19" s="7">
+      <c r="M19" s="6">
         <v>11000</v>
       </c>
     </row>
@@ -1558,7 +1561,7 @@
       <c r="H20">
         <v>9999999</v>
       </c>
-      <c r="I20" s="7">
+      <c r="I20" s="6">
         <v>11000</v>
       </c>
       <c r="J20">
@@ -1570,7 +1573,7 @@
       <c r="L20">
         <v>9999999</v>
       </c>
-      <c r="M20" s="7">
+      <c r="M20" s="6">
         <v>11000</v>
       </c>
     </row>
@@ -1599,7 +1602,7 @@
       <c r="H21">
         <v>9999999</v>
       </c>
-      <c r="I21" s="7">
+      <c r="I21" s="6">
         <v>11000</v>
       </c>
       <c r="J21">
@@ -1611,7 +1614,7 @@
       <c r="L21">
         <v>9999999</v>
       </c>
-      <c r="M21" s="7">
+      <c r="M21" s="6">
         <v>11000</v>
       </c>
     </row>
@@ -1640,7 +1643,7 @@
       <c r="H22">
         <v>9999999</v>
       </c>
-      <c r="I22" s="7">
+      <c r="I22" s="6">
         <v>11000</v>
       </c>
       <c r="J22">
@@ -1652,7 +1655,7 @@
       <c r="L22">
         <v>9999999</v>
       </c>
-      <c r="M22" s="7">
+      <c r="M22" s="6">
         <v>11000</v>
       </c>
     </row>
@@ -1681,7 +1684,7 @@
       <c r="H23">
         <v>9999999</v>
       </c>
-      <c r="I23" s="7">
+      <c r="I23" s="6">
         <v>11000</v>
       </c>
       <c r="J23">
@@ -1693,7 +1696,7 @@
       <c r="L23">
         <v>9999999</v>
       </c>
-      <c r="M23" s="7">
+      <c r="M23" s="6">
         <v>11000</v>
       </c>
     </row>
@@ -1722,7 +1725,7 @@
       <c r="H24">
         <v>9999999</v>
       </c>
-      <c r="I24" s="7">
+      <c r="I24" s="6">
         <v>11000</v>
       </c>
       <c r="J24">
@@ -1734,7 +1737,7 @@
       <c r="L24">
         <v>9999999</v>
       </c>
-      <c r="M24" s="7">
+      <c r="M24" s="6">
         <v>11000</v>
       </c>
     </row>
@@ -1763,7 +1766,7 @@
       <c r="H25">
         <v>9999999</v>
       </c>
-      <c r="I25" s="7">
+      <c r="I25" s="6">
         <v>11000</v>
       </c>
       <c r="J25">
@@ -1775,7 +1778,7 @@
       <c r="L25">
         <v>9999999</v>
       </c>
-      <c r="M25" s="7">
+      <c r="M25" s="6">
         <v>11000</v>
       </c>
     </row>
@@ -1804,7 +1807,7 @@
       <c r="H26">
         <v>9999999</v>
       </c>
-      <c r="I26" s="7">
+      <c r="I26" s="6">
         <v>11000</v>
       </c>
       <c r="J26">
@@ -1816,7 +1819,7 @@
       <c r="L26">
         <v>9999999</v>
       </c>
-      <c r="M26" s="7">
+      <c r="M26" s="6">
         <v>11000</v>
       </c>
     </row>
@@ -1845,7 +1848,7 @@
       <c r="H27">
         <v>9999999</v>
       </c>
-      <c r="I27" s="7">
+      <c r="I27" s="6">
         <v>11000</v>
       </c>
       <c r="J27">
@@ -1857,7 +1860,7 @@
       <c r="L27">
         <v>9999999</v>
       </c>
-      <c r="M27" s="7">
+      <c r="M27" s="6">
         <v>11000</v>
       </c>
     </row>
@@ -1886,7 +1889,7 @@
       <c r="H28">
         <v>9999999</v>
       </c>
-      <c r="I28" s="7">
+      <c r="I28" s="6">
         <v>11000</v>
       </c>
       <c r="J28">
@@ -1898,7 +1901,7 @@
       <c r="L28">
         <v>9999999</v>
       </c>
-      <c r="M28" s="7">
+      <c r="M28" s="6">
         <v>11000</v>
       </c>
     </row>
@@ -1921,59 +1924,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" s="5"/>
+      <c r="A3" s="4"/>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" s="5"/>
+      <c r="A4" s="4"/>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" s="5"/>
+      <c r="A5" s="4"/>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" s="5"/>
+      <c r="A6" s="4"/>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" s="5"/>
+      <c r="A7" s="4"/>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" s="5"/>
+      <c r="A8" s="4"/>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" s="5"/>
+      <c r="A9" s="4"/>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A10" s="5"/>
+      <c r="A10" s="4"/>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A11" s="5"/>
+      <c r="A11" s="4"/>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A12" s="5"/>
+      <c r="A12" s="4"/>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A13" s="5"/>
+      <c r="A13" s="4"/>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A14" s="5"/>
+      <c r="A14" s="4"/>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A15" s="5"/>
+      <c r="A15" s="4"/>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A16" s="5"/>
+      <c r="A16" s="4"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" s="5"/>
+      <c r="A17" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -1985,7 +1988,7 @@
   <dimension ref="A1:E325"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2000,10 +2003,10 @@
       <c r="B1" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>32</v>
       </c>
       <c r="E1" t="s">
@@ -7525,10 +7528,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71493739-45C2-4A8D-9266-24BB3FC8F4DB}">
-  <dimension ref="A1:T18"/>
+  <dimension ref="A1:U18"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="W7" sqref="W7"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="U1" sqref="U1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7544,35 +7547,35 @@
     <col min="20" max="20" width="20.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="5" t="s">
         <v>10</v>
       </c>
       <c r="K1" s="1" t="s">
@@ -7581,95 +7584,101 @@
       <c r="L1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="M1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="N1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="O1" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="P1" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="Q1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="R1" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="S1" s="6" t="s">
+      <c r="S1" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="T1" s="6" t="s">
+      <c r="T1" s="5" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+      <c r="U1" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="7">
+      <c r="B2" s="6">
         <v>260000</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C2" s="6">
         <v>40000</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D2" s="6">
         <v>25</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2" s="6">
         <v>0.25</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2" s="6">
         <v>0</v>
       </c>
-      <c r="G2" s="7">
+      <c r="G2" s="6">
         <v>1500</v>
       </c>
-      <c r="H2" s="7">
+      <c r="H2" s="6">
         <v>0</v>
       </c>
-      <c r="I2" s="7">
+      <c r="I2" s="6">
         <v>0.37409999999999999</v>
       </c>
-      <c r="J2" s="7">
+      <c r="J2" s="6">
         <v>0.38879999999999998</v>
       </c>
-      <c r="K2" s="7">
+      <c r="K2" s="6">
         <v>0.8</v>
       </c>
-      <c r="L2" s="7">
+      <c r="L2" s="6">
         <v>0.8</v>
       </c>
       <c r="M2">
         <v>25</v>
       </c>
-      <c r="N2" s="7">
+      <c r="N2" s="6">
         <v>5</v>
       </c>
-      <c r="O2" s="7">
+      <c r="O2" s="6">
         <v>5</v>
       </c>
-      <c r="P2" s="7">
+      <c r="P2" s="6">
         <v>70</v>
       </c>
-      <c r="Q2" s="7">
+      <c r="Q2" s="6">
         <v>70</v>
       </c>
-      <c r="R2" s="7">
+      <c r="R2" s="6">
         <v>0.85</v>
       </c>
-      <c r="S2" s="7">
+      <c r="S2" s="6">
         <v>0.2</v>
       </c>
-      <c r="T2" s="7">
+      <c r="T2" s="6">
         <v>100000</v>
       </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+      <c r="U2" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
         <v>31</v>
       </c>
       <c r="B3">
@@ -7681,57 +7690,60 @@
       <c r="D3">
         <v>50</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="6">
         <v>0.25</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="6">
         <v>0</v>
       </c>
-      <c r="G3" s="7">
+      <c r="G3" s="6">
         <v>6000</v>
       </c>
-      <c r="H3" s="7">
+      <c r="H3" s="6">
         <v>0</v>
       </c>
-      <c r="I3" s="7">
+      <c r="I3" s="6">
         <v>7.2700000000000001E-2</v>
       </c>
-      <c r="J3" s="7">
+      <c r="J3" s="6">
         <v>7.2700000000000001E-2</v>
       </c>
-      <c r="K3" s="7">
+      <c r="K3" s="6">
         <v>0.8</v>
       </c>
-      <c r="L3" s="7">
+      <c r="L3" s="6">
         <v>0.8</v>
       </c>
       <c r="M3">
         <v>15</v>
       </c>
-      <c r="N3" s="7">
+      <c r="N3" s="6">
         <v>5</v>
       </c>
-      <c r="O3" s="7">
+      <c r="O3" s="6">
         <v>5</v>
       </c>
-      <c r="P3" s="7">
+      <c r="P3" s="6">
         <v>10000</v>
       </c>
-      <c r="Q3" s="7">
+      <c r="Q3" s="6">
         <v>10000</v>
       </c>
-      <c r="R3" s="7">
+      <c r="R3" s="6">
         <v>0.7</v>
       </c>
-      <c r="S3" s="7">
+      <c r="S3" s="6">
         <v>0.2</v>
       </c>
-      <c r="T3" s="7">
+      <c r="T3" s="6">
         <v>25000</v>
       </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
+      <c r="U3" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
         <v>41</v>
       </c>
       <c r="B4">
@@ -7743,10 +7755,10 @@
       <c r="D4">
         <v>50</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="6">
         <v>0.25</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F4" s="6">
         <v>0</v>
       </c>
       <c r="G4">
@@ -7755,84 +7767,87 @@
       <c r="H4">
         <v>0</v>
       </c>
-      <c r="I4" s="7">
+      <c r="I4" s="6">
         <v>7.2700000000000001E-2</v>
       </c>
-      <c r="J4" s="7">
+      <c r="J4" s="6">
         <v>7.2700000000000001E-2</v>
       </c>
-      <c r="K4" s="7">
+      <c r="K4" s="6">
         <v>0.8</v>
       </c>
-      <c r="L4" s="7">
+      <c r="L4" s="6">
         <v>0.8</v>
       </c>
-      <c r="M4" s="7">
+      <c r="M4" s="6">
         <v>20</v>
       </c>
-      <c r="N4" s="7">
+      <c r="N4" s="6">
         <v>5</v>
       </c>
-      <c r="O4" s="7">
+      <c r="O4" s="6">
         <v>5</v>
       </c>
-      <c r="P4" s="7">
+      <c r="P4" s="6">
         <v>10000</v>
       </c>
-      <c r="Q4" s="7">
+      <c r="Q4" s="6">
         <v>10000</v>
       </c>
-      <c r="R4" s="7">
+      <c r="R4" s="6">
         <v>0.7</v>
       </c>
-      <c r="S4" s="7">
+      <c r="S4" s="6">
         <v>0.2</v>
       </c>
-      <c r="T4" s="7">
+      <c r="T4" s="6">
         <v>25000</v>
       </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A5" s="5"/>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A6" s="5"/>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A7" s="5"/>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A8" s="5"/>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A9" s="5"/>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A10" s="5"/>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A11" s="5"/>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A12" s="5"/>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A13" s="5"/>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A14" s="5"/>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A15" s="5"/>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A16" s="5"/>
+      <c r="U4" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A5" s="4"/>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A6" s="4"/>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A7" s="4"/>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A8" s="4"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A9" s="4"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A10" s="4"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A11" s="4"/>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A12" s="4"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A13" s="4"/>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A14" s="4"/>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A15" s="4"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A16" s="4"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" s="5"/>
+      <c r="A17" s="4"/>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" s="5"/>
+      <c r="A18" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -7854,16 +7869,16 @@
       <c r="A1" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E1" s="5"/>
+      <c r="E1" s="4"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
@@ -8262,16 +8277,16 @@
       <c r="A1" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E1" s="5"/>
+      <c r="E1" s="4"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
@@ -8660,8 +8675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3790A601-26C3-4DCA-97B6-9342C547A4A0}">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8670,23 +8685,23 @@
       <c r="A1" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E1" s="5"/>
+      <c r="E1" s="4"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2024</v>
       </c>
-      <c r="B2" s="4">
-        <v>150000</v>
+      <c r="B2" s="3">
+        <v>65000</v>
       </c>
       <c r="C2">
         <v>13333</v>
@@ -8699,8 +8714,8 @@
       <c r="A3">
         <v>2025</v>
       </c>
-      <c r="B3" s="4">
-        <v>93020</v>
+      <c r="B3" s="3">
+        <v>65000</v>
       </c>
       <c r="C3">
         <v>13333</v>
@@ -8713,8 +8728,8 @@
       <c r="A4">
         <v>2026</v>
       </c>
-      <c r="B4" s="4">
-        <v>93020</v>
+      <c r="B4" s="3">
+        <v>65000</v>
       </c>
       <c r="C4">
         <v>13333</v>
@@ -8727,8 +8742,8 @@
       <c r="A5">
         <v>2027</v>
       </c>
-      <c r="B5" s="4">
-        <v>93020</v>
+      <c r="B5" s="3">
+        <v>65000</v>
       </c>
       <c r="C5">
         <v>13333</v>
@@ -8741,8 +8756,8 @@
       <c r="A6">
         <v>2028</v>
       </c>
-      <c r="B6" s="4">
-        <v>93020</v>
+      <c r="B6" s="3">
+        <v>65000</v>
       </c>
       <c r="C6">
         <v>13333</v>
@@ -8755,8 +8770,8 @@
       <c r="A7">
         <v>2029</v>
       </c>
-      <c r="B7" s="4">
-        <v>93020</v>
+      <c r="B7" s="3">
+        <v>65000</v>
       </c>
       <c r="C7">
         <v>13333</v>
@@ -8769,8 +8784,8 @@
       <c r="A8">
         <v>2030</v>
       </c>
-      <c r="B8" s="4">
-        <v>93020</v>
+      <c r="B8" s="3">
+        <v>65000</v>
       </c>
       <c r="C8">
         <v>20000</v>
@@ -8783,8 +8798,8 @@
       <c r="A9">
         <v>2031</v>
       </c>
-      <c r="B9" s="4">
-        <v>61911.5</v>
+      <c r="B9" s="3">
+        <v>65000</v>
       </c>
       <c r="C9">
         <v>20000</v>
@@ -8797,8 +8812,8 @@
       <c r="A10">
         <v>2032</v>
       </c>
-      <c r="B10" s="4">
-        <v>61911.5</v>
+      <c r="B10" s="3">
+        <v>65000</v>
       </c>
       <c r="C10">
         <v>20000</v>
@@ -8811,8 +8826,8 @@
       <c r="A11">
         <v>2033</v>
       </c>
-      <c r="B11" s="4">
-        <v>61911.5</v>
+      <c r="B11" s="3">
+        <v>65000</v>
       </c>
       <c r="C11">
         <v>20000</v>
@@ -8825,8 +8840,8 @@
       <c r="A12">
         <v>2034</v>
       </c>
-      <c r="B12" s="4">
-        <v>61911.5</v>
+      <c r="B12" s="3">
+        <v>65000</v>
       </c>
       <c r="C12">
         <v>20000</v>
@@ -8839,8 +8854,8 @@
       <c r="A13">
         <v>2035</v>
       </c>
-      <c r="B13" s="4">
-        <v>61911.5</v>
+      <c r="B13" s="3">
+        <v>65000</v>
       </c>
       <c r="C13">
         <v>20000</v>
@@ -8853,8 +8868,8 @@
       <c r="A14">
         <v>2036</v>
       </c>
-      <c r="B14" s="4">
-        <v>61911.5</v>
+      <c r="B14" s="3">
+        <v>65000</v>
       </c>
       <c r="C14">
         <v>20000</v>
@@ -8867,8 +8882,8 @@
       <c r="A15">
         <v>2037</v>
       </c>
-      <c r="B15" s="4">
-        <v>61911.5</v>
+      <c r="B15" s="3">
+        <v>65000</v>
       </c>
       <c r="C15">
         <v>20000</v>
@@ -8881,8 +8896,8 @@
       <c r="A16">
         <v>2038</v>
       </c>
-      <c r="B16" s="4">
-        <v>61911.5</v>
+      <c r="B16" s="3">
+        <v>65000</v>
       </c>
       <c r="C16">
         <v>20000</v>
@@ -8895,8 +8910,8 @@
       <c r="A17">
         <v>2039</v>
       </c>
-      <c r="B17" s="4">
-        <v>61911.5</v>
+      <c r="B17" s="3">
+        <v>65000</v>
       </c>
       <c r="C17">
         <v>20000</v>
@@ -8909,8 +8924,8 @@
       <c r="A18">
         <v>2040</v>
       </c>
-      <c r="B18" s="4">
-        <v>61911.5</v>
+      <c r="B18" s="3">
+        <v>65000</v>
       </c>
       <c r="C18">
         <v>20000</v>
@@ -8923,8 +8938,8 @@
       <c r="A19">
         <v>2041</v>
       </c>
-      <c r="B19" s="4">
-        <v>57655.199999999997</v>
+      <c r="B19" s="3">
+        <v>65000</v>
       </c>
       <c r="C19">
         <v>20000</v>
@@ -8937,8 +8952,8 @@
       <c r="A20">
         <v>2042</v>
       </c>
-      <c r="B20" s="4">
-        <v>57655.199999999997</v>
+      <c r="B20" s="3">
+        <v>65000</v>
       </c>
       <c r="C20">
         <v>20000</v>
@@ -8951,8 +8966,8 @@
       <c r="A21">
         <v>2043</v>
       </c>
-      <c r="B21" s="4">
-        <v>57655.199999999997</v>
+      <c r="B21" s="3">
+        <v>65000</v>
       </c>
       <c r="C21">
         <v>20000</v>
@@ -8966,7 +8981,7 @@
         <v>2044</v>
       </c>
       <c r="B22" s="3">
-        <v>57655.199999999997</v>
+        <v>65000</v>
       </c>
       <c r="C22">
         <v>20000</v>
@@ -8980,7 +8995,7 @@
         <v>2045</v>
       </c>
       <c r="B23" s="3">
-        <v>57655.199999999997</v>
+        <v>65000</v>
       </c>
       <c r="C23">
         <v>20000</v>
@@ -8994,7 +9009,7 @@
         <v>2046</v>
       </c>
       <c r="B24" s="3">
-        <v>57655.199999999997</v>
+        <v>65000</v>
       </c>
       <c r="C24">
         <v>20000</v>
@@ -9008,7 +9023,7 @@
         <v>2047</v>
       </c>
       <c r="B25" s="3">
-        <v>57655.199999999997</v>
+        <v>65000</v>
       </c>
       <c r="C25">
         <v>20000</v>
@@ -9022,7 +9037,7 @@
         <v>2048</v>
       </c>
       <c r="B26" s="3">
-        <v>57655.199999999997</v>
+        <v>65000</v>
       </c>
       <c r="C26">
         <v>20000</v>
@@ -9036,7 +9051,7 @@
         <v>2049</v>
       </c>
       <c r="B27" s="3">
-        <v>57655.199999999997</v>
+        <v>65000</v>
       </c>
       <c r="C27">
         <v>20000</v>
@@ -9050,7 +9065,7 @@
         <v>2050</v>
       </c>
       <c r="B28" s="3">
-        <v>57655.199999999997</v>
+        <v>65000</v>
       </c>
       <c r="C28">
         <v>20000</v>

</xml_diff>

<commit_message>
Adding init's to constraints with y0 exceptions
</commit_message>
<xml_diff>
--- a/Input_urbsextensionv1.xlsx
+++ b/Input_urbsextensionv1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxoi\GitHub\urbs-extension\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D88DD8F-3C38-47CA-A616-17733F889E38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24541DE1-766E-4CDE-B596-0030E3ACB1DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-5445" windowWidth="38640" windowHeight="21120" activeTab="4" xr2:uid="{81864710-3A67-40FC-ABA1-4EF02E4F8A12}"/>
+    <workbookView xWindow="67080" yWindow="-1935" windowWidth="29040" windowHeight="17520" activeTab="7" xr2:uid="{81864710-3A67-40FC-ABA1-4EF02E4F8A12}"/>
   </bookViews>
   <sheets>
     <sheet name="Base" sheetId="10" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="49">
   <si>
     <t>Value</t>
   </si>
@@ -187,6 +187,9 @@
   </si>
   <si>
     <t>Initial_secondary_cap</t>
+  </si>
+  <si>
+    <t>price_reduction_init</t>
   </si>
 </sst>
 </file>
@@ -7528,10 +7531,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71493739-45C2-4A8D-9266-24BB3FC8F4DB}">
-  <dimension ref="A1:U18"/>
+  <dimension ref="A1:V18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="U1" sqref="U1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7547,7 +7550,7 @@
     <col min="20" max="20" width="20.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>18</v>
       </c>
@@ -7611,8 +7614,11 @@
       <c r="U1" s="5" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V1" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>27</v>
       </c>
@@ -7676,8 +7682,11 @@
       <c r="U2" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V2" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>31</v>
       </c>
@@ -7741,8 +7750,11 @@
       <c r="U3" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V3" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>41</v>
       </c>
@@ -7806,41 +7818,44 @@
       <c r="U4" s="6">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="V4" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
@@ -8675,8 +8690,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3790A601-26C3-4DCA-97B6-9342C547A4A0}">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Defines power variation parameters
Defines power variation parameters for different learning rates.
This prepares the code for using these parameters in subsequent
calculations.
</commit_message>
<xml_diff>
--- a/Input_urbsextensionv1.xlsx
+++ b/Input_urbsextensionv1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxoi\GitHub\urbs-extension\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00CDBADA-B079-48EC-B15F-74FCE604A884}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6FA9B08-323D-4013-A62E-287D8C61B49C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="67080" yWindow="-1935" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{81864710-3A67-40FC-ABA1-4EF02E4F8A12}"/>
+    <workbookView xWindow="67080" yWindow="-1935" windowWidth="29040" windowHeight="17520" activeTab="4" xr2:uid="{81864710-3A67-40FC-ABA1-4EF02E4F8A12}"/>
   </bookViews>
   <sheets>
     <sheet name="Base" sheetId="10" r:id="rId1"/>
@@ -783,8 +783,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6185AF38-42FD-4CFF-B287-2FCFFF6C6EF3}">
   <dimension ref="A1:Q28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8887,8 +8887,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71493739-45C2-4A8D-9266-24BB3FC8F4DB}">
   <dimension ref="A1:Z18"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9019,7 +9019,7 @@
         <v>0.8</v>
       </c>
       <c r="L2" s="5">
-        <v>0.8</v>
+        <v>0.2</v>
       </c>
       <c r="M2">
         <v>25</v>

</xml_diff>